<commit_message>
pesi e closest counterfactual
</commit_message>
<xml_diff>
--- a/statistiche/counterfactualsRandomForest.xlsx
+++ b/statistiche/counterfactualsRandomForest.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,77 +436,77 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>ER Triage</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Release D</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>IV Liquid</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Release B</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Leucocytes</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Release C</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ER Sepsis Triage</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Admission IC</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>IV Antibiotics</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>LacticAcid</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ER Registration</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Admission NC</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Release A</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>CRP</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Release D</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>ER Sepsis Triage</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Admission IC</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>LacticAcid</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>ER Triage</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>IV Liquid</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Admission NC</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Release A</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Leucocytes</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Release C</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Release B</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>ER Registration</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>IV Antibiotics</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
@@ -528,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -537,10 +537,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -549,19 +549,19 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" t="n">
         <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
         <v>1</v>
@@ -585,19 +585,19 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -606,19 +606,19 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
         <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="N3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
         <v>1</v>
@@ -629,120 +629,6 @@
         </is>
       </c>
       <c r="Q3" t="inlineStr">
-        <is>
-          <t>Counterfactual</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>9</v>
-      </c>
-      <c r="J4" t="n">
-        <v>5</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" t="n">
-        <v>1</v>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>regular</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Counterfactual</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>27</v>
-      </c>
-      <c r="J5" t="n">
-        <v>29</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" t="n">
-        <v>1</v>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>regular</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
         <is>
           <t>Counterfactual</t>
         </is>

</xml_diff>